<commit_message>
Added excelsheet to framework
</commit_message>
<xml_diff>
--- a/src/test/java/com/sapizon/instavr/testData/testdata.xlsx
+++ b/src/test/java/com/sapizon/instavr/testData/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/InstaVR/src/test/java/com/sapizon/instavr/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Test_Case</t>
-  </si>
-  <si>
-    <t>Run_Mode</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>pramodnp.pnp@gmail.com</t>
+  </si>
+  <si>
+    <t>pramodnp1995</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -45,12 +57,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,20 +363,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extracting data from excel sheet
extracting user name and password from excel sheet
</commit_message>
<xml_diff>
--- a/src/test/java/com/sapizon/instavr/testData/testdata.xlsx
+++ b/src/test/java/com/sapizon/instavr/testData/testdata.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="8320" yWindow="2400" windowWidth="17000" windowHeight="12480" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="testcase" sheetId="1" r:id="rId1"/>
+    <sheet name="loginTestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -366,7 +366,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>